<commit_message>
[DOC] : System Workbench manual - update
</commit_message>
<xml_diff>
--- a/STM32 System Workbench Manual.xlsx
+++ b/STM32 System Workbench Manual.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="program DL" sheetId="1" r:id="rId1"/>
     <sheet name="Install" sheetId="2" r:id="rId2"/>
     <sheet name="사용법" sheetId="3" r:id="rId3"/>
+    <sheet name="CubeMX" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>http://www.openstm32.org/System%2BWorkbench%2Bfor%2BSTM32</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -155,6 +156,14 @@
   </si>
   <si>
     <t>4. Compile - Project &gt; Build All를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 설치된 IDE에 맞춰 Toolchain/IDE를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System Workbench를 사용하는 경우, SW4STM32를 선택한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1644,6 +1653,109 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>618280</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>132505</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="그룹 3"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="981075" y="704850"/>
+          <a:ext cx="6761905" cy="6761905"/>
+          <a:chOff x="981075" y="704850"/>
+          <a:chExt cx="6761905" cy="6761905"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="2" name="그림 1"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="981075" y="704850"/>
+            <a:ext cx="6761905" cy="6761905"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="모서리가 둥근 직사각형 2"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1285875" y="3124199"/>
+            <a:ext cx="3057525" cy="523875"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
@@ -1687,7 +1799,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1722,7 +1834,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1933,7 +2045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
@@ -2010,7 +2122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C324"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
@@ -2128,8 +2240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="R77" sqref="R77"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2168,4 +2280,35 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C3"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="4" width="5.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>